<commit_message>
Code Review 2 Contribution Spreadsheet
</commit_message>
<xml_diff>
--- a/individual_assessment_group_4.xlsx
+++ b/individual_assessment_group_4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeahe\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabeth/Downloads/SEM-Group-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E63CD80-F22C-4B2B-AFF9-EF209A33ED1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D7E456-E87B-074C-ABD6-3A810DB3F821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4669A0B8-2A04-4C8A-A346-B743537D3B7F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{4669A0B8-2A04-4C8A-A346-B743537D3B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Matriculation Number</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Individual Assessment Group 4</t>
+  </si>
+  <si>
+    <t>17.5%</t>
+  </si>
+  <si>
+    <t>16.5%</t>
   </si>
 </sst>
 </file>
@@ -137,29 +143,29 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,95 +484,109 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>40643354</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>0.2</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>40606309</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>0.2</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>40646750</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>0.2</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>40647491</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>0.2</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>40545326</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>0.2</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>40626955</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>0</v>
       </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>